<commit_message>
Atualizado IDF e ICP
</commit_message>
<xml_diff>
--- a/outputs/sisaprophelper#autoaprop/autoapropxlsx/ICP.XLSX
+++ b/outputs/sisaprophelper#autoaprop/autoapropxlsx/ICP.XLSX
@@ -159,6 +159,9 @@
     <t>JOSE DAMIAO CASTANHO FARIA</t>
   </si>
   <si>
+    <t>GUILHERME LEMOS MOURAO</t>
+  </si>
+  <si>
     <t>ADILSON GERARDO BARROS AMARAL</t>
   </si>
   <si>
@@ -237,9 +240,6 @@
     <t> </t>
   </si>
   <si>
-    <t> </t>
-  </si>
-  <si>
     <t>2984</t>
   </si>
   <si>
@@ -249,6 +249,9 @@
     <t>3558</t>
   </si>
   <si>
+    <t>3575</t>
+  </si>
+  <si>
     <t>3756</t>
   </si>
   <si>
@@ -262,9 +265,6 @@
   </si>
   <si>
     <t>4211</t>
-  </si>
-  <si>
-    <t> </t>
   </si>
   <si>
     <t> </t>

</xml_diff>

<commit_message>
Mudanças ID --> IG / IE / IC / IQ
</commit_message>
<xml_diff>
--- a/outputs/sisaprophelper#autoaprop/autoapropxlsx/ICP.XLSX
+++ b/outputs/sisaprophelper#autoaprop/autoapropxlsx/ICP.XLSX
@@ -180,9 +180,6 @@
     <t>MARCELO L. SANTANA DE CAMPOS</t>
   </si>
   <si>
-    <t>ADILSON GERARDO BARROS AMARAL</t>
-  </si>
-  <si>
     <t>DEBORA SILVA DE SOUZA VACCARI</t>
   </si>
   <si>
@@ -240,6 +237,9 @@
     <t> </t>
   </si>
   <si>
+    <t> </t>
+  </si>
+  <si>
     <t>475</t>
   </si>
   <si>
@@ -270,9 +270,6 @@
     <t>3750</t>
   </si>
   <si>
-    <t>3756</t>
-  </si>
-  <si>
     <t>3929</t>
   </si>
   <si>
@@ -298,6 +295,9 @@
   </si>
   <si>
     <t>4211</t>
+  </si>
+  <si>
+    <t> </t>
   </si>
   <si>
     <t> </t>

</xml_diff>